<commit_message>
Commit with additional excel docs and calculations
</commit_message>
<xml_diff>
--- a/raw-data/strong.xlsx
+++ b/raw-data/strong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\russia_strong\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0848EAC-BD19-4D92-A081-0B93D1B75145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C099BF-9909-42C0-8456-49D3210D722D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7BD05E0B-31D4-4FCC-B52C-BC4E7F8EB199}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
   <si>
     <t>Statistic</t>
   </si>
@@ -80,40 +80,13 @@
     <t>Military Exp. As Share of U.S.</t>
   </si>
   <si>
-    <t>Russia National Power</t>
-  </si>
-  <si>
     <t>Pct Change</t>
   </si>
   <si>
-    <t>Saudi Arabia National Power</t>
-  </si>
-  <si>
-    <t>Nigeria National Power</t>
-  </si>
-  <si>
-    <t>Ukraine National Power</t>
-  </si>
-  <si>
-    <t>Brazil National Power</t>
-  </si>
-  <si>
-    <t>India National Power</t>
-  </si>
-  <si>
-    <t>China National Power</t>
-  </si>
-  <si>
-    <t>South Africa National Power</t>
-  </si>
-  <si>
-    <t>United Kingdom National Power</t>
-  </si>
-  <si>
-    <t>United States National Power</t>
-  </si>
-  <si>
-    <t>Germany National Power</t>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Russia</t>
   </si>
 </sst>
 </file>
@@ -488,605 +461,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CE4597-B9D6-46A3-8505-012A63183B6C}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>2018</v>
-      </c>
       <c r="C2">
+        <v>2018</v>
+      </c>
+      <c r="D2">
         <v>144477860</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2019</v>
-      </c>
       <c r="C3">
+        <v>2019</v>
+      </c>
+      <c r="D3">
         <v>144373535</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>-6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>2018</v>
-      </c>
       <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4">
         <v>3915637487520.0181</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>2019</v>
-      </c>
       <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5">
         <v>3968180465310.3721</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2018</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="1">
         <v>61387.546980435385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>2019</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="C7">
+        <v>2019</v>
+      </c>
+      <c r="D7" s="1">
         <v>64144.260676602898</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>2018</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="C8">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="2">
         <v>1.9029999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>2019</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="C9">
+        <v>2019</v>
+      </c>
+      <c r="D9" s="3">
         <v>1.881E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>-1.1299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>2018</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="C10">
+        <v>2018</v>
+      </c>
+      <c r="D10" s="3">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>2019</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="D11" s="3">
         <v>3.0519999999999999E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>-1.55E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>2018</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="C12">
+        <v>2018</v>
+      </c>
+      <c r="D12" s="3">
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="B13">
-        <v>2019</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="C13">
+        <v>2019</v>
+      </c>
+      <c r="D13" s="3">
         <v>3.3509999999999998E-2</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="B14">
-        <v>2018</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="C14">
+        <v>2018</v>
+      </c>
+      <c r="D14" s="4">
         <v>0.10373761400000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="B15">
-        <v>2019</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="C15">
+        <v>2019</v>
+      </c>
+      <c r="D15" s="4">
         <v>0.1032925</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
-        <v>2018</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="C16">
+        <v>2018</v>
+      </c>
+      <c r="D16" s="4">
         <v>0.442250957</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="B17">
-        <v>2019</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="C17">
+        <v>2019</v>
+      </c>
+      <c r="D17" s="4">
         <v>0.43984200000000001</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>-5.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="B18">
-        <v>2018</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="C18">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="4">
         <v>0.1844412</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
-        <v>2019</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="C19">
+        <v>2019</v>
+      </c>
+      <c r="D19" s="4">
         <v>0.1761556</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
-        <v>2018</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="C20">
+        <v>2018</v>
+      </c>
+      <c r="D20" s="4">
         <v>0.1952372</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
-        <v>2019</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="C21">
+        <v>2019</v>
+      </c>
+      <c r="D21" s="4">
         <v>0.19334519999999999</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>-9.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="B22">
-        <v>2018</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="C22">
+        <v>2018</v>
+      </c>
+      <c r="D22" s="4">
         <v>0.24216799999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="B23">
-        <v>2019</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="C23">
+        <v>2019</v>
+      </c>
+      <c r="D23" s="4">
         <v>0.24074000000000001</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>-5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="B24">
-        <v>2018</v>
-      </c>
-      <c r="C24" s="4">
+      <c r="C24">
+        <v>2018</v>
+      </c>
+      <c r="D24" s="4">
         <v>8.9946300000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
         <v>14</v>
       </c>
-      <c r="B25">
-        <v>2019</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="C25">
+        <v>2019</v>
+      </c>
+      <c r="D25" s="4">
         <v>8.9249999999999996E-2</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="3">
         <v>-7.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>2018</v>
-      </c>
-      <c r="C26" s="4">
-        <v>7.58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>2019</v>
-      </c>
-      <c r="C27" s="4">
-        <v>7.56</v>
-      </c>
-      <c r="D27" s="3">
-        <v>-2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28">
-        <v>2018</v>
-      </c>
-      <c r="C28" s="4">
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29">
-        <v>2019</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2.42</v>
-      </c>
-      <c r="D29" s="3">
-        <v>-9.9599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30">
-        <v>2018</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31">
-        <v>2019</v>
-      </c>
-      <c r="C31" s="4">
-        <v>1.54</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3.8999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32">
-        <v>2018</v>
-      </c>
-      <c r="C32">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>2019</v>
-      </c>
-      <c r="C33">
-        <v>0.63</v>
-      </c>
-      <c r="D33" s="3">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>2018</v>
-      </c>
-      <c r="C34">
-        <v>4.83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35">
-        <v>2019</v>
-      </c>
-      <c r="C35">
-        <v>4.78</v>
-      </c>
-      <c r="D35" s="3">
-        <v>-9.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36">
-        <v>2018</v>
-      </c>
-      <c r="C36">
-        <v>11.39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37">
-        <v>2019</v>
-      </c>
-      <c r="C37">
-        <v>11.5</v>
-      </c>
-      <c r="D37" s="3">
-        <v>9.2999999999999992E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38">
-        <v>2018</v>
-      </c>
-      <c r="C38">
-        <v>21.55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39">
-        <v>2019</v>
-      </c>
-      <c r="C39">
-        <v>21.83</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1.3299999999999999E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40">
-        <v>2018</v>
-      </c>
-      <c r="C40">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41">
-        <v>2019</v>
-      </c>
-      <c r="C41">
-        <v>0.92</v>
-      </c>
-      <c r="D41" s="3">
-        <v>-1.11E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42">
-        <v>2018</v>
-      </c>
-      <c r="C42">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43">
-        <v>2019</v>
-      </c>
-      <c r="C43">
-        <v>2.42</v>
-      </c>
-      <c r="D43" s="3">
-        <v>-2.01E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44">
-        <v>2018</v>
-      </c>
-      <c r="C44">
-        <v>24.07</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45">
-        <v>2019</v>
-      </c>
-      <c r="C45">
-        <v>24.23</v>
-      </c>
-      <c r="D45" s="3">
-        <v>6.6E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46">
-        <v>2018</v>
-      </c>
-      <c r="C46">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47">
-        <v>2019</v>
-      </c>
-      <c r="C47">
-        <v>3.06</v>
-      </c>
-      <c r="D47" s="3">
-        <v>3.0999999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>